<commit_message>
Apparently the last save didn't save, trying again.
</commit_message>
<xml_diff>
--- a/resources/SAMM_spreadsheet.xlsx
+++ b/resources/SAMM_spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brian\projects\toolbox-spreadsheet\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{292BC4B7-7B12-4347-AC37-4172A4AAFB02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B808CE-3672-45DD-B358-61FE064D1F36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Attribution and License" sheetId="1" r:id="rId1"/>
@@ -11879,6 +11879,9 @@
       <rgbColor rgb="00333399"/>
       <rgbColor rgb="00333333"/>
     </indexedColors>
+    <mruColors>
+      <color rgb="FFFFC221"/>
+    </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -20847,7 +20850,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:Z230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="B7" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="I227" sqref="I227:I228"/>
     </sheetView>
   </sheetViews>
@@ -29524,14 +29527,14 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:Z144"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A49" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="J54" sqref="J54"/>
+    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.36328125" style="284" customWidth="1"/>
-    <col min="2" max="2" width="23.81640625" style="284" customWidth="1"/>
+    <col min="1" max="1" width="14.90625" style="284" customWidth="1"/>
+    <col min="2" max="2" width="24.81640625" style="284" customWidth="1"/>
     <col min="3" max="3" width="9.1796875" style="284" customWidth="1"/>
     <col min="4" max="6" width="6.6328125" style="284" customWidth="1"/>
     <col min="7" max="7" width="15" style="284" hidden="1" customWidth="1"/>
@@ -29539,8 +29542,8 @@
     <col min="9" max="10" width="15" style="284" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.36328125" style="284" customWidth="1"/>
     <col min="12" max="14" width="15" style="284" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.6328125" style="284" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="22.1796875" style="284" customWidth="1"/>
+    <col min="20" max="20" width="14.7265625" style="284" customWidth="1"/>
+    <col min="21" max="21" width="24.6328125" style="284" customWidth="1"/>
     <col min="22" max="22" width="10.1796875" style="284" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="10.453125" style="284" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="10.453125" style="284" customWidth="1"/>
@@ -34061,23 +34064,23 @@
       <c r="L93" s="303"/>
       <c r="M93" s="303"/>
       <c r="N93" s="303"/>
-      <c r="V93" t="str">
+      <c r="V93" s="305" t="str">
         <f>T94</f>
         <v>Governance</v>
       </c>
-      <c r="W93" t="str">
+      <c r="W93" s="305" t="str">
         <f>T97</f>
         <v>Design</v>
       </c>
-      <c r="X93" t="str">
+      <c r="X93" s="305" t="str">
         <f>T100</f>
         <v>Implementation</v>
       </c>
-      <c r="Y93" t="str">
+      <c r="Y93" s="305" t="str">
         <f>T103</f>
         <v>Verification</v>
       </c>
-      <c r="Z93" t="str">
+      <c r="Z93" s="305" t="str">
         <f>T106</f>
         <v>Operations</v>
       </c>
@@ -35778,7 +35781,7 @@
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="3"/>
-        <color rgb="FFBDBF17"/>
+        <color rgb="FFFFC221"/>
       </dataBar>
     </cfRule>
   </conditionalFormatting>
@@ -35814,7 +35817,7 @@
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
-        <color rgb="FFBDBF17"/>
+        <color rgb="FFFFC221"/>
       </dataBar>
     </cfRule>
   </conditionalFormatting>
@@ -35877,7 +35880,7 @@
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="3"/>
-        <color rgb="FFBDBF17"/>
+        <color rgb="FFFFC221"/>
       </dataBar>
     </cfRule>
   </conditionalFormatting>
@@ -35922,7 +35925,7 @@
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="3"/>
-        <color rgb="FFBDBF17"/>
+        <color rgb="FFFFC221"/>
       </dataBar>
     </cfRule>
   </conditionalFormatting>
@@ -35967,7 +35970,7 @@
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="3"/>
-        <color rgb="FFBDBF17"/>
+        <color rgb="FFFFC221"/>
       </dataBar>
     </cfRule>
   </conditionalFormatting>
@@ -35994,7 +35997,7 @@
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
-        <color rgb="FFBDBF17"/>
+        <color rgb="FFFFC221"/>
       </dataBar>
     </cfRule>
   </conditionalFormatting>
@@ -36048,7 +36051,7 @@
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
-        <color rgb="FFBDBF17"/>
+        <color rgb="FFFFC221"/>
       </dataBar>
     </cfRule>
   </conditionalFormatting>
@@ -36057,7 +36060,7 @@
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
-        <color rgb="FFBDBF17"/>
+        <color rgb="FFFFC221"/>
       </dataBar>
     </cfRule>
   </conditionalFormatting>
@@ -36066,7 +36069,7 @@
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
-        <color rgb="FFBDBF17"/>
+        <color rgb="FFFFC221"/>
       </dataBar>
     </cfRule>
   </conditionalFormatting>
@@ -36219,7 +36222,7 @@
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
-        <color rgb="FFBDBF17"/>
+        <color rgb="FFFFC221"/>
       </dataBar>
     </cfRule>
   </conditionalFormatting>
@@ -36228,7 +36231,7 @@
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
-        <color rgb="FFBDBF17"/>
+        <color rgb="FFFFC221"/>
       </dataBar>
     </cfRule>
   </conditionalFormatting>
@@ -36237,7 +36240,7 @@
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
-        <color rgb="FFBDBF17"/>
+        <color rgb="FFFFC221"/>
       </dataBar>
     </cfRule>
   </conditionalFormatting>
@@ -36305,8 +36308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Y154"/>
   <sheetViews>
-    <sheetView topLeftCell="B82" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J102" sqref="J102"/>
+    <sheetView tabSelected="1" topLeftCell="B121" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M148" sqref="M148:M154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -36317,16 +36320,17 @@
     <col min="4" max="4" width="68" style="130" customWidth="1"/>
     <col min="5" max="5" width="5.1796875" style="143" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="39" style="25" customWidth="1"/>
-    <col min="7" max="7" width="8.6328125" style="21" customWidth="1"/>
-    <col min="8" max="8" width="8.6328125" style="117" customWidth="1"/>
+    <col min="7" max="7" width="8.6328125" style="21" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="8.6328125" style="117" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="15" style="11" customWidth="1"/>
     <col min="10" max="10" width="36.6328125" style="284" customWidth="1"/>
-    <col min="11" max="11" width="7" style="284" customWidth="1"/>
-    <col min="12" max="12" width="9.1796875" style="284" customWidth="1"/>
+    <col min="11" max="11" width="7" style="284" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="9.1796875" style="284" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="16.453125" style="284" customWidth="1"/>
     <col min="14" max="14" width="49.81640625" style="284" customWidth="1"/>
-    <col min="15" max="15" width="28.6328125" style="284" customWidth="1"/>
-    <col min="16" max="17" width="15" style="284" customWidth="1"/>
+    <col min="15" max="15" width="28.6328125" style="284" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="15" style="284" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="15" style="284" customWidth="1"/>
     <col min="18" max="18" width="36.1796875" style="284" customWidth="1"/>
     <col min="19" max="20" width="15" style="284" hidden="1" customWidth="1"/>
     <col min="21" max="21" width="15" style="284" customWidth="1"/>
@@ -48637,7 +48641,7 @@
       <formula>K98&lt;G98</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="5">
+  <dataValidations disablePrompts="1" count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F18:F20 F22:F24 F27:F29 F31:F33 F36:F38 F40:F42 F46:F48 F50:F52 F55:F57 F59:F61 F64:F66 F68:F70 F74:F76 F78:F80 F83:F85 F87:F89 F92:F94 F96:F98 F102:F104 F106:F108 F111:F113 F115:F117 F120:F122 F124:F126 F130:F132 F134:F136 F139:F141 F143:F145 F148:F150 F152:F154" xr:uid="{89F0B844-4463-A141-8363-D064AC2726DD}">
       <formula1>INDIRECT("Ans"&amp;INDIRECT("RC[-1]",0))</formula1>
     </dataValidation>
@@ -48666,8 +48670,8 @@
   </sheetPr>
   <dimension ref="A1:AE132"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="L35" sqref="L35"/>
+    <sheetView topLeftCell="A6" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
@@ -51330,7 +51334,7 @@
     <mergeCell ref="S9:T9"/>
     <mergeCell ref="U9:V9"/>
   </mergeCells>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation showInputMessage="1" showErrorMessage="1" sqref="B12:B26" xr:uid="{00000000-0002-0000-0400-000000000000}"/>
   </dataValidations>
   <pageMargins left="0.55118110236220474" right="0.55118110236220474" top="0.39370078740157483" bottom="0.39370078740157483" header="0.51181102362204722" footer="0.51181102362204722"/>

</xml_diff>